<commit_message>
Adjusted some dates in the EventList and drafted the codebook for the first tab
</commit_message>
<xml_diff>
--- a/admin/event_sampling/btmobile25a_EventList.xlsx
+++ b/admin/event_sampling/btmobile25a_EventList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ncoles/Documents/GitHub/btmobile/admin/event_sampling/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtaka\Documents\GitHub\btmobile\admin\event_sampling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB32394-7245-404F-909E-36A478EF89AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0BD901F-2567-40D2-BFED-CD0767A835D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="32000" windowHeight="17500" xr2:uid="{AD4E61A8-FDF9-BC48-9383-4A13CF80A2B5}"/>
+    <workbookView xWindow="38280" yWindow="-3165" windowWidth="25440" windowHeight="15270" xr2:uid="{AD4E61A8-FDF9-BC48-9383-4A13CF80A2B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2196" uniqueCount="653">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2211" uniqueCount="665">
   <si>
     <t>Event Name</t>
   </si>
@@ -1999,6 +1999,42 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>April 28 2001</t>
+  </si>
+  <si>
+    <t>August 4 2018</t>
+  </si>
+  <si>
+    <t>February 1 2016</t>
+  </si>
+  <si>
+    <t>August 17 2012</t>
+  </si>
+  <si>
+    <t>March 15 2003</t>
+  </si>
+  <si>
+    <t>December 17 2017</t>
+  </si>
+  <si>
+    <t>WHO declares International Health emergency</t>
+  </si>
+  <si>
+    <t>August 8 2014</t>
+  </si>
+  <si>
+    <t>June 1 2014</t>
+  </si>
+  <si>
+    <t>July 1 2019</t>
+  </si>
+  <si>
+    <t>July 20 2011</t>
+  </si>
+  <si>
+    <t>Global oil price drop</t>
   </si>
 </sst>
 </file>
@@ -2914,18 +2950,18 @@
   <dimension ref="A1:O112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="A1:K106"/>
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="42.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" customWidth="1"/>
+    <col min="2" max="2" width="40.5" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" customWidth="1"/>
     <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2964,7 +3000,7 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2996,7 +3032,7 @@
         <v>732.06896549999999</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -3028,7 +3064,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -3063,7 +3099,7 @@
         <v>374.1935484</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -3095,7 +3131,7 @@
         <v>373.64</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -3127,7 +3163,7 @@
         <v>371.75</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -3159,7 +3195,7 @@
         <v>333.4</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -3191,7 +3227,7 @@
         <v>198.33333329999999</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -3223,7 +3259,7 @@
         <v>192.58333329999999</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>58</v>
       </c>
@@ -3255,7 +3291,7 @@
         <v>150.66666670000001</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>63</v>
       </c>
@@ -3287,7 +3323,7 @@
         <v>125.16666669999999</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>69</v>
       </c>
@@ -3319,7 +3355,7 @@
         <v>93.92307692</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>74</v>
       </c>
@@ -3351,7 +3387,7 @@
         <v>82.212643679999999</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>80</v>
       </c>
@@ -3383,7 +3419,7 @@
         <v>70.092307689999998</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>86</v>
       </c>
@@ -3393,9 +3429,6 @@
       <c r="C15" t="s">
         <v>88</v>
       </c>
-      <c r="D15" t="s">
-        <v>88</v>
-      </c>
       <c r="E15" t="s">
         <v>89</v>
       </c>
@@ -3418,7 +3451,7 @@
         <v>61.446153850000002</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>92</v>
       </c>
@@ -3428,8 +3461,8 @@
       <c r="C16" t="s">
         <v>94</v>
       </c>
-      <c r="D16" s="2">
-        <v>45704</v>
+      <c r="D16" s="2" t="s">
+        <v>655</v>
       </c>
       <c r="E16" t="s">
         <v>95</v>
@@ -3453,7 +3486,7 @@
         <v>52.433155079999999</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>98</v>
       </c>
@@ -3485,7 +3518,7 @@
         <v>38.024390240000002</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>104</v>
       </c>
@@ -3495,8 +3528,8 @@
       <c r="C18" t="s">
         <v>106</v>
       </c>
-      <c r="D18" s="2">
-        <v>45881</v>
+      <c r="D18" s="2" t="s">
+        <v>656</v>
       </c>
       <c r="E18" t="s">
         <v>107</v>
@@ -3520,7 +3553,7 @@
         <v>31.38356164</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>110</v>
       </c>
@@ -3530,8 +3563,8 @@
       <c r="C19" t="s">
         <v>112</v>
       </c>
-      <c r="D19" s="2">
-        <v>45719</v>
+      <c r="D19" s="2" t="s">
+        <v>657</v>
       </c>
       <c r="E19" t="s">
         <v>113</v>
@@ -3555,7 +3588,7 @@
         <v>26.13839286</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>116</v>
       </c>
@@ -3587,7 +3620,7 @@
         <v>24.8</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>122</v>
       </c>
@@ -3619,7 +3652,7 @@
         <v>21.704724410000001</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>128</v>
       </c>
@@ -3651,7 +3684,7 @@
         <v>17.571428569999998</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>133</v>
       </c>
@@ -3683,7 +3716,7 @@
         <v>15.289908260000001</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>138</v>
       </c>
@@ -3715,7 +3748,7 @@
         <v>13.29032258</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>144</v>
       </c>
@@ -3747,7 +3780,7 @@
         <v>11.27737226</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>150</v>
       </c>
@@ -3757,8 +3790,8 @@
       <c r="C26" t="s">
         <v>152</v>
       </c>
-      <c r="D26" s="2">
-        <v>46008</v>
+      <c r="D26" s="2" t="s">
+        <v>658</v>
       </c>
       <c r="E26" t="s">
         <v>153</v>
@@ -3782,7 +3815,7 @@
         <v>10.741427249999999</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>156</v>
       </c>
@@ -3792,9 +3825,6 @@
       <c r="C27" t="s">
         <v>158</v>
       </c>
-      <c r="D27" t="s">
-        <v>158</v>
-      </c>
       <c r="E27" t="s">
         <v>159</v>
       </c>
@@ -3817,7 +3847,7 @@
         <v>9.4833272260000001</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>162</v>
       </c>
@@ -3849,7 +3879,7 @@
         <v>9.461538462</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>168</v>
       </c>
@@ -3859,11 +3889,11 @@
       <c r="C29" t="s">
         <v>170</v>
       </c>
-      <c r="D29" s="2">
-        <v>45883</v>
+      <c r="D29" s="2" t="s">
+        <v>660</v>
       </c>
       <c r="E29" t="s">
-        <v>95</v>
+        <v>659</v>
       </c>
       <c r="F29" t="s">
         <v>171</v>
@@ -3884,7 +3914,7 @@
         <v>9.4278169009999999</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>173</v>
       </c>
@@ -3916,7 +3946,7 @@
         <v>7.4210526320000003</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>179</v>
       </c>
@@ -3948,7 +3978,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>184</v>
       </c>
@@ -3980,7 +4010,7 @@
         <v>7.1666666670000003</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>190</v>
       </c>
@@ -4012,7 +4042,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>196</v>
       </c>
@@ -4044,7 +4074,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>202</v>
       </c>
@@ -4076,7 +4106,7 @@
         <v>6.8421052629999997</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>207</v>
       </c>
@@ -4108,7 +4138,7 @@
         <v>5.6666666670000003</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>212</v>
       </c>
@@ -4140,7 +4170,7 @@
         <v>5.4341463409999999</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>218</v>
       </c>
@@ -4172,7 +4202,7 @@
         <v>5.0028715000000004</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>224</v>
       </c>
@@ -4204,7 +4234,7 @@
         <v>4.9090909089999997</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>229</v>
       </c>
@@ -4239,7 +4269,7 @@
         <v>4.9050809600000003</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>235</v>
       </c>
@@ -4274,7 +4304,7 @@
         <v>4.8840579709999998</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>241</v>
       </c>
@@ -4309,7 +4339,7 @@
         <v>4.4124168509999997</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>248</v>
       </c>
@@ -4341,7 +4371,7 @@
         <v>4.1982507289999997</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
         <v>254</v>
       </c>
@@ -4373,7 +4403,7 @@
         <v>4.0868644070000002</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
         <v>260</v>
       </c>
@@ -4405,7 +4435,7 @@
         <v>4.0077519380000002</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
         <v>266</v>
       </c>
@@ -4437,7 +4467,7 @@
         <v>3.9310344829999999</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
         <v>272</v>
       </c>
@@ -4447,8 +4477,8 @@
       <c r="C47" t="s">
         <v>274</v>
       </c>
-      <c r="D47" s="2">
-        <v>45822</v>
+      <c r="D47" s="2" t="s">
+        <v>661</v>
       </c>
       <c r="E47" t="s">
         <v>275</v>
@@ -4472,7 +4502,7 @@
         <v>3.6413934430000001</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
         <v>278</v>
       </c>
@@ -4504,7 +4534,7 @@
         <v>3.5825825830000002</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
         <v>284</v>
       </c>
@@ -4539,7 +4569,7 @@
         <v>3.404090268</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
         <v>290</v>
       </c>
@@ -4571,7 +4601,7 @@
         <v>3.1278608480000001</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
         <v>296</v>
       </c>
@@ -4603,7 +4633,7 @@
         <v>3.074449666</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
         <v>302</v>
       </c>
@@ -4635,7 +4665,7 @@
         <v>2.9500594530000002</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
         <v>308</v>
       </c>
@@ -4667,7 +4697,7 @@
         <v>2.7332754129999999</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
         <v>314</v>
       </c>
@@ -4699,7 +4729,7 @@
         <v>2.6666666669999999</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A55" t="s">
         <v>320</v>
       </c>
@@ -4731,7 +4761,7 @@
         <v>2.626415094</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
         <v>325</v>
       </c>
@@ -4766,7 +4796,7 @@
         <v>2.5333993069999998</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
         <v>332</v>
       </c>
@@ -4798,7 +4828,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
         <v>337</v>
       </c>
@@ -4830,7 +4860,7 @@
         <v>2.3918918919999999</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A59" t="s">
         <v>342</v>
       </c>
@@ -4862,7 +4892,7 @@
         <v>2.3608815430000001</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A60" t="s">
         <v>347</v>
       </c>
@@ -4894,7 +4924,7 @@
         <v>2.2122905030000002</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A61" t="s">
         <v>352</v>
       </c>
@@ -4904,8 +4934,8 @@
       <c r="C61" t="s">
         <v>354</v>
       </c>
-      <c r="D61" s="2">
-        <v>45748</v>
+      <c r="D61" s="2" t="s">
+        <v>653</v>
       </c>
       <c r="E61" t="s">
         <v>355</v>
@@ -4929,7 +4959,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A62" t="s">
         <v>358</v>
       </c>
@@ -4964,7 +4994,7 @@
         <v>2.1497619920000002</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A63" t="s">
         <v>363</v>
       </c>
@@ -4974,8 +5004,8 @@
       <c r="C63" t="s">
         <v>365</v>
       </c>
-      <c r="D63" s="2">
-        <v>45857</v>
+      <c r="D63" s="2" t="s">
+        <v>662</v>
       </c>
       <c r="E63" t="s">
         <v>366</v>
@@ -4999,7 +5029,7 @@
         <v>2.1182795699999999</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A64" t="s">
         <v>368</v>
       </c>
@@ -5031,7 +5061,7 @@
         <v>2.0744466799999999</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A65" t="s">
         <v>374</v>
       </c>
@@ -5066,7 +5096,7 @@
         <v>2.0208877279999999</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
         <v>381</v>
       </c>
@@ -5098,7 +5128,7 @@
         <v>1.9797297300000001</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
         <v>385</v>
       </c>
@@ -5130,7 +5160,7 @@
         <v>1.97254902</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A68" t="s">
         <v>391</v>
       </c>
@@ -5163,7 +5193,7 @@
       </c>
       <c r="L68" s="3"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A69" t="s">
         <v>397</v>
       </c>
@@ -5173,8 +5203,8 @@
       <c r="C69" t="s">
         <v>399</v>
       </c>
-      <c r="D69" s="2">
-        <v>45849</v>
+      <c r="D69" s="2" t="s">
+        <v>663</v>
       </c>
       <c r="E69" t="s">
         <v>400</v>
@@ -5198,7 +5228,7 @@
         <v>1.8958333329999999</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A70" t="s">
         <v>403</v>
       </c>
@@ -5233,7 +5263,7 @@
         <v>1.8885779700000001</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A71" t="s">
         <v>410</v>
       </c>
@@ -5263,7 +5293,7 @@
       </c>
       <c r="L71" s="3"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A72" t="s">
         <v>415</v>
       </c>
@@ -5295,7 +5325,7 @@
         <v>1.7983193280000001</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A73" t="s">
         <v>421</v>
       </c>
@@ -5330,7 +5360,7 @@
         <v>1.5984147950000001</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A74" t="s">
         <v>428</v>
       </c>
@@ -5362,7 +5392,7 @@
         <v>1.579150579</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A75" t="s">
         <v>434</v>
       </c>
@@ -5394,7 +5424,7 @@
         <v>1.568181818</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A76" t="s">
         <v>439</v>
       </c>
@@ -5426,7 +5456,7 @@
         <v>1.435647584</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A77" t="s">
         <v>445</v>
       </c>
@@ -5436,11 +5466,11 @@
       <c r="C77" t="s">
         <v>447</v>
       </c>
-      <c r="D77">
-        <v>2010</v>
+      <c r="D77" t="s">
+        <v>661</v>
       </c>
       <c r="E77" t="s">
-        <v>448</v>
+        <v>664</v>
       </c>
       <c r="F77" t="s">
         <v>449</v>
@@ -5452,16 +5482,17 @@
         <v>46100</v>
       </c>
       <c r="I77">
-        <v>3307</v>
+        <v>4929</v>
       </c>
       <c r="J77">
-        <v>4635</v>
+        <v>6002</v>
       </c>
       <c r="K77">
-        <v>1.4015724220000001</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+        <f>J77/I77</f>
+        <v>1.2176912152566444</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A78" t="s">
         <v>451</v>
       </c>
@@ -5493,7 +5524,7 @@
         <v>1.3647798739999999</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A79" t="s">
         <v>455</v>
       </c>
@@ -5525,7 +5556,7 @@
         <v>1.3508403360000001</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A80" t="s">
         <v>461</v>
       </c>
@@ -5557,7 +5588,7 @@
         <v>1.34034824</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A81" t="s">
         <v>467</v>
       </c>
@@ -5592,7 +5623,7 @@
         <v>1.2913669059999999</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A82" t="s">
         <v>473</v>
       </c>
@@ -5627,7 +5658,7 @@
         <v>1.259629101</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A83" t="s">
         <v>479</v>
       </c>
@@ -5659,7 +5690,7 @@
         <v>1.25433526</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A84" t="s">
         <v>485</v>
       </c>
@@ -5669,8 +5700,8 @@
       <c r="C84" t="s">
         <v>487</v>
       </c>
-      <c r="D84" s="2">
-        <v>45887</v>
+      <c r="D84" s="2" t="s">
+        <v>654</v>
       </c>
       <c r="E84" t="s">
         <v>488</v>
@@ -5694,7 +5725,7 @@
         <v>1.2402420569999999</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A85" t="s">
         <v>491</v>
       </c>
@@ -5726,7 +5757,7 @@
         <v>1.2215113950000001</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A86" t="s">
         <v>497</v>
       </c>
@@ -5758,7 +5789,7 @@
         <v>1.203136137</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A87" t="s">
         <v>503</v>
       </c>
@@ -5790,7 +5821,7 @@
         <v>1.136022514</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A88" t="s">
         <v>508</v>
       </c>
@@ -5822,7 +5853,7 @@
         <v>1.1282633369999999</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A89" t="s">
         <v>514</v>
       </c>
@@ -5854,7 +5885,7 @@
         <v>1.124572211</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A90" t="s">
         <v>520</v>
       </c>
@@ -5883,7 +5914,7 @@
         <v>1.0699300700000001</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A91" t="s">
         <v>525</v>
       </c>
@@ -5912,7 +5943,7 @@
         <v>1.0052083329999999</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A92" t="s">
         <v>530</v>
       </c>
@@ -5947,7 +5978,7 @@
         <v>0.82306752699999997</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A93" t="s">
         <v>535</v>
       </c>
@@ -5976,7 +6007,7 @@
         <v>0.15762273900000001</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A94" t="s">
         <v>540</v>
       </c>
@@ -5987,7 +6018,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A95" t="s">
         <v>543</v>
       </c>
@@ -5995,7 +6026,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A96" t="s">
         <v>545</v>
       </c>
@@ -6015,7 +6046,7 @@
         <v>70080</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A97" t="s">
         <v>550</v>
       </c>
@@ -6035,7 +6066,7 @@
         <v>14330</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A98" t="s">
         <v>555</v>
       </c>
@@ -6055,7 +6086,7 @@
         <v>11970</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A99" t="s">
         <v>559</v>
       </c>
@@ -6075,7 +6106,7 @@
         <v>5926</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A100" t="s">
         <v>563</v>
       </c>
@@ -6095,7 +6126,7 @@
         <v>3730</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A101" t="s">
         <v>568</v>
       </c>
@@ -6115,7 +6146,7 @@
         <v>3126</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A102" t="s">
         <v>572</v>
       </c>
@@ -6135,7 +6166,7 @@
         <v>1879</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A103" t="s">
         <v>577</v>
       </c>
@@ -6155,7 +6186,7 @@
         <v>1673</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A104" t="s">
         <v>582</v>
       </c>
@@ -6175,7 +6206,7 @@
         <v>1437</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A105" t="s">
         <v>585</v>
       </c>
@@ -6195,7 +6226,7 @@
         <v>1184</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A106" t="s">
         <v>589</v>
       </c>
@@ -6209,12 +6240,12 @@
         <v>592</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A109" t="s">
         <v>593</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A110" t="s">
         <v>594</v>
       </c>
@@ -6240,7 +6271,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A111" t="s">
         <v>598</v>
       </c>
@@ -6263,7 +6294,7 @@
         <v>1252</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A112" t="s">
         <v>602</v>
       </c>
@@ -6297,10 +6328,10 @@
   <dimension ref="A1:G110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="42.5" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="79.33203125" style="5" bestFit="1" customWidth="1"/>
@@ -6311,7 +6342,7 @@
     <col min="8" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -6334,7 +6365,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -6354,7 +6385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
         <v>17</v>
       </c>
@@ -6374,7 +6405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="5" t="s">
         <v>23</v>
       </c>
@@ -6394,7 +6425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="5" t="s">
         <v>30</v>
       </c>
@@ -6414,7 +6445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
         <v>35</v>
       </c>
@@ -6434,7 +6465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" s="5" t="s">
         <v>41</v>
       </c>
@@ -6454,7 +6485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
         <v>47</v>
       </c>
@@ -6474,7 +6505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
         <v>53</v>
       </c>
@@ -6494,7 +6525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" s="5" t="s">
         <v>58</v>
       </c>
@@ -6514,7 +6545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="32" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
         <v>63</v>
       </c>
@@ -6534,7 +6565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" s="5" t="s">
         <v>69</v>
       </c>
@@ -6554,7 +6585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" s="5" t="s">
         <v>74</v>
       </c>
@@ -6574,7 +6605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="32" x14ac:dyDescent="0.4">
       <c r="A14" s="5" t="s">
         <v>80</v>
       </c>
@@ -6594,7 +6625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" s="5" t="s">
         <v>86</v>
       </c>
@@ -6614,7 +6645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" s="5" t="s">
         <v>92</v>
       </c>
@@ -6634,7 +6665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A17" s="5" t="s">
         <v>98</v>
       </c>
@@ -6654,7 +6685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A18" s="5" t="s">
         <v>104</v>
       </c>
@@ -6674,7 +6705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A19" s="5" t="s">
         <v>110</v>
       </c>
@@ -6694,7 +6725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A20" s="5" t="s">
         <v>116</v>
       </c>
@@ -6714,7 +6745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A21" s="5" t="s">
         <v>122</v>
       </c>
@@ -6734,7 +6765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A22" s="5" t="s">
         <v>128</v>
       </c>
@@ -6754,7 +6785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A23" s="5" t="s">
         <v>133</v>
       </c>
@@ -6774,7 +6805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="32" x14ac:dyDescent="0.4">
       <c r="A24" s="5" t="s">
         <v>138</v>
       </c>
@@ -6794,7 +6825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="32" x14ac:dyDescent="0.4">
       <c r="A25" s="5" t="s">
         <v>144</v>
       </c>
@@ -6814,7 +6845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A26" s="5" t="s">
         <v>150</v>
       </c>
@@ -6834,7 +6865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A27" s="5" t="s">
         <v>156</v>
       </c>
@@ -6854,7 +6885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A28" s="5" t="s">
         <v>162</v>
       </c>
@@ -6874,7 +6905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A29" s="5" t="s">
         <v>168</v>
       </c>
@@ -6894,7 +6925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A30" s="5" t="s">
         <v>173</v>
       </c>
@@ -6914,7 +6945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A31" s="5" t="s">
         <v>179</v>
       </c>
@@ -6934,7 +6965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A32" s="5" t="s">
         <v>184</v>
       </c>
@@ -6954,7 +6985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A33" s="5" t="s">
         <v>190</v>
       </c>
@@ -6974,7 +7005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="96" x14ac:dyDescent="0.4">
       <c r="A34" s="5" t="s">
         <v>196</v>
       </c>
@@ -6997,7 +7028,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A35" s="5" t="s">
         <v>202</v>
       </c>
@@ -7017,7 +7048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A36" s="5" t="s">
         <v>207</v>
       </c>
@@ -7037,7 +7068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A37" s="5" t="s">
         <v>212</v>
       </c>
@@ -7057,7 +7088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" ht="32" x14ac:dyDescent="0.4">
       <c r="A38" s="5" t="s">
         <v>218</v>
       </c>
@@ -7077,7 +7108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A39" s="5" t="s">
         <v>224</v>
       </c>
@@ -7097,7 +7128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A40" s="5" t="s">
         <v>229</v>
       </c>
@@ -7117,7 +7148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A41" s="5" t="s">
         <v>235</v>
       </c>
@@ -7137,7 +7168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A42" s="5" t="s">
         <v>241</v>
       </c>
@@ -7157,7 +7188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A43" s="5" t="s">
         <v>248</v>
       </c>
@@ -7177,7 +7208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" ht="64" x14ac:dyDescent="0.4">
       <c r="A44" s="5" t="s">
         <v>254</v>
       </c>
@@ -7197,7 +7228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A45" s="5" t="s">
         <v>260</v>
       </c>
@@ -7217,7 +7248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A46" s="5" t="s">
         <v>266</v>
       </c>
@@ -7237,7 +7268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A47" s="5" t="s">
         <v>272</v>
       </c>
@@ -7257,7 +7288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A48" s="5" t="s">
         <v>278</v>
       </c>
@@ -7277,7 +7308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A49" s="5" t="s">
         <v>284</v>
       </c>
@@ -7297,7 +7328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A50" s="5" t="s">
         <v>290</v>
       </c>
@@ -7317,7 +7348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A51" s="5" t="s">
         <v>296</v>
       </c>
@@ -7337,7 +7368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A52" s="5" t="s">
         <v>302</v>
       </c>
@@ -7357,7 +7388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A53" s="5" t="s">
         <v>308</v>
       </c>
@@ -7377,7 +7408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A54" s="5" t="s">
         <v>314</v>
       </c>
@@ -7397,7 +7428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A55" s="5" t="s">
         <v>320</v>
       </c>
@@ -7417,7 +7448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" ht="32" x14ac:dyDescent="0.4">
       <c r="A56" s="5" t="s">
         <v>325</v>
       </c>
@@ -7437,7 +7468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A57" s="5" t="s">
         <v>332</v>
       </c>
@@ -7457,7 +7488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A58" s="5" t="s">
         <v>337</v>
       </c>
@@ -7477,7 +7508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A59" s="5" t="s">
         <v>342</v>
       </c>
@@ -7497,7 +7528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A60" s="5" t="s">
         <v>347</v>
       </c>
@@ -7517,7 +7548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A61" s="5" t="s">
         <v>352</v>
       </c>
@@ -7537,7 +7568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A62" s="5" t="s">
         <v>358</v>
       </c>
@@ -7557,7 +7588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A63" s="5" t="s">
         <v>363</v>
       </c>
@@ -7577,7 +7608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A64" s="5" t="s">
         <v>368</v>
       </c>
@@ -7597,7 +7628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A65" s="5" t="s">
         <v>374</v>
       </c>
@@ -7617,7 +7648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A66" s="5" t="s">
         <v>381</v>
       </c>
@@ -7637,7 +7668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A67" s="5" t="s">
         <v>385</v>
       </c>
@@ -7657,7 +7688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A68" s="5" t="s">
         <v>391</v>
       </c>
@@ -7677,7 +7708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A69" s="5" t="s">
         <v>397</v>
       </c>
@@ -7697,7 +7728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A70" s="5" t="s">
         <v>403</v>
       </c>
@@ -7717,7 +7748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" ht="48" x14ac:dyDescent="0.4">
       <c r="A71" s="5" t="s">
         <v>410</v>
       </c>
@@ -7737,7 +7768,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A72" s="5" t="s">
         <v>415</v>
       </c>
@@ -7757,7 +7788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A73" s="5" t="s">
         <v>421</v>
       </c>
@@ -7777,7 +7808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A74" s="5" t="s">
         <v>428</v>
       </c>
@@ -7797,7 +7828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A75" s="5" t="s">
         <v>434</v>
       </c>
@@ -7817,7 +7848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A76" s="5" t="s">
         <v>439</v>
       </c>
@@ -7837,7 +7868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A77" s="5" t="s">
         <v>445</v>
       </c>
@@ -7857,7 +7888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A78" s="5" t="s">
         <v>451</v>
       </c>
@@ -7877,7 +7908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A79" s="5" t="s">
         <v>455</v>
       </c>
@@ -7897,7 +7928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A80" s="5" t="s">
         <v>461</v>
       </c>
@@ -7917,7 +7948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A81" s="5" t="s">
         <v>467</v>
       </c>
@@ -7937,7 +7968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A82" s="5" t="s">
         <v>473</v>
       </c>
@@ -7957,7 +7988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A83" s="5" t="s">
         <v>479</v>
       </c>
@@ -7977,7 +8008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" ht="32" x14ac:dyDescent="0.4">
       <c r="A84" s="5" t="s">
         <v>485</v>
       </c>
@@ -7997,7 +8028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A85" s="5" t="s">
         <v>491</v>
       </c>
@@ -8017,7 +8048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" ht="48" x14ac:dyDescent="0.4">
       <c r="A86" s="5" t="s">
         <v>497</v>
       </c>
@@ -8040,7 +8071,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A87" s="5" t="s">
         <v>503</v>
       </c>
@@ -8060,7 +8091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" ht="64" x14ac:dyDescent="0.4">
       <c r="A88" s="5" t="s">
         <v>508</v>
       </c>
@@ -8083,7 +8114,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A89" s="5" t="s">
         <v>514</v>
       </c>
@@ -8103,7 +8134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" ht="32" x14ac:dyDescent="0.4">
       <c r="A90" s="5" t="s">
         <v>520</v>
       </c>
@@ -8120,7 +8151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A91" s="5" t="s">
         <v>525</v>
       </c>
@@ -8137,7 +8168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A92" s="5" t="s">
         <v>530</v>
       </c>
@@ -8157,7 +8188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A93" s="5" t="s">
         <v>535</v>
       </c>
@@ -8174,7 +8205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A94" s="5" t="s">
         <v>540</v>
       </c>
@@ -8191,7 +8222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="153" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" ht="144" x14ac:dyDescent="0.4">
       <c r="A95" s="5" t="s">
         <v>543</v>
       </c>
@@ -8208,7 +8239,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" ht="48" x14ac:dyDescent="0.4">
       <c r="A96" s="5" t="s">
         <v>545</v>
       </c>
@@ -8228,7 +8259,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A97" s="5" t="s">
         <v>550</v>
       </c>
@@ -8245,7 +8276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A98" s="5" t="s">
         <v>555</v>
       </c>
@@ -8265,7 +8296,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A99" s="5" t="s">
         <v>559</v>
       </c>
@@ -8285,7 +8316,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7" ht="112" x14ac:dyDescent="0.4">
       <c r="A100" s="5" t="s">
         <v>563</v>
       </c>
@@ -8305,7 +8336,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A101" s="5" t="s">
         <v>568</v>
       </c>
@@ -8322,7 +8353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A102" s="5" t="s">
         <v>572</v>
       </c>
@@ -8339,7 +8370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7" ht="48" x14ac:dyDescent="0.4">
       <c r="A103" s="5" t="s">
         <v>577</v>
       </c>
@@ -8359,7 +8390,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A104" s="5" t="s">
         <v>582</v>
       </c>
@@ -8379,7 +8410,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A105" s="5" t="s">
         <v>585</v>
       </c>
@@ -8399,7 +8430,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A106" s="5" t="s">
         <v>589</v>
       </c>
@@ -8419,7 +8450,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.4">
       <c r="C110" s="6"/>
     </row>
   </sheetData>
@@ -8431,17 +8462,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90E5CAFD-27E0-BE46-8D5E-79A93373063C}">
   <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A106" sqref="A106"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="K77" sqref="K77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="10.83203125" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8479,7 +8510,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -8511,7 +8542,7 @@
         <v>732.06896549999999</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -8543,7 +8574,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -8578,7 +8609,7 @@
         <v>374.1935484</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -8610,7 +8641,7 @@
         <v>373.64</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -8642,7 +8673,7 @@
         <v>371.75</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -8674,7 +8705,7 @@
         <v>333.4</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -8706,7 +8737,7 @@
         <v>198.33333329999999</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -8738,7 +8769,7 @@
         <v>192.58333329999999</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>58</v>
       </c>
@@ -8773,7 +8804,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>63</v>
       </c>
@@ -8805,7 +8836,7 @@
         <v>125.16666669999999</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>69</v>
       </c>
@@ -8837,7 +8868,7 @@
         <v>93.92307692</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>74</v>
       </c>
@@ -8869,7 +8900,7 @@
         <v>82.212643679999999</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>80</v>
       </c>
@@ -8901,7 +8932,7 @@
         <v>70.092307689999998</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>86</v>
       </c>
@@ -8936,7 +8967,7 @@
         <v>61.446153850000002</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>92</v>
       </c>
@@ -8971,7 +9002,7 @@
         <v>52.433155079999999</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>98</v>
       </c>
@@ -9003,7 +9034,7 @@
         <v>38.024390240000002</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>104</v>
       </c>
@@ -9038,7 +9069,7 @@
         <v>31.38356164</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>110</v>
       </c>
@@ -9073,7 +9104,7 @@
         <v>26.13839286</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>116</v>
       </c>
@@ -9108,7 +9139,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>122</v>
       </c>
@@ -9140,7 +9171,7 @@
         <v>21.704724410000001</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>128</v>
       </c>
@@ -9172,7 +9203,7 @@
         <v>17.571428569999998</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>133</v>
       </c>
@@ -9204,7 +9235,7 @@
         <v>15.289908260000001</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>138</v>
       </c>
@@ -9236,7 +9267,7 @@
         <v>13.29032258</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>144</v>
       </c>
@@ -9268,7 +9299,7 @@
         <v>11.27737226</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>150</v>
       </c>
@@ -9303,7 +9334,7 @@
         <v>10.741427249999999</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>156</v>
       </c>
@@ -9338,7 +9369,7 @@
         <v>9.4833272260000001</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>162</v>
       </c>
@@ -9370,7 +9401,7 @@
         <v>9.461538462</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>168</v>
       </c>
@@ -9405,7 +9436,7 @@
         <v>9.4278169009999999</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>173</v>
       </c>
@@ -9440,7 +9471,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>179</v>
       </c>
@@ -9475,7 +9506,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>184</v>
       </c>
@@ -9510,7 +9541,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>190</v>
       </c>
@@ -9545,7 +9576,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>196</v>
       </c>
@@ -9580,7 +9611,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>202</v>
       </c>
@@ -9615,7 +9646,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>207</v>
       </c>
@@ -9647,7 +9678,7 @@
         <v>5.6666666670000003</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>212</v>
       </c>
@@ -9679,7 +9710,7 @@
         <v>5.4341463409999999</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>218</v>
       </c>
@@ -9711,7 +9742,7 @@
         <v>5.0028715000000004</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>224</v>
       </c>
@@ -9746,7 +9777,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>229</v>
       </c>
@@ -9784,7 +9815,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>235</v>
       </c>
@@ -9822,7 +9853,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>241</v>
       </c>
@@ -9857,7 +9888,7 @@
         <v>4.4124168509999997</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>248</v>
       </c>
@@ -9889,7 +9920,7 @@
         <v>4.1982507289999997</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
         <v>254</v>
       </c>
@@ -9921,7 +9952,7 @@
         <v>4.0868644070000002</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
         <v>260</v>
       </c>
@@ -9953,7 +9984,7 @@
         <v>4.0077519380000002</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
         <v>266</v>
       </c>
@@ -9988,7 +10019,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
         <v>272</v>
       </c>
@@ -10023,7 +10054,7 @@
         <v>3.6413934430000001</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
         <v>278</v>
       </c>
@@ -10055,7 +10086,7 @@
         <v>3.5825825830000002</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
         <v>284</v>
       </c>
@@ -10090,7 +10121,7 @@
         <v>3.404090268</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
         <v>290</v>
       </c>
@@ -10122,7 +10153,7 @@
         <v>3.1278608480000001</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
         <v>296</v>
       </c>
@@ -10154,7 +10185,7 @@
         <v>3.074449666</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
         <v>302</v>
       </c>
@@ -10186,7 +10217,7 @@
         <v>2.9500594530000002</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
         <v>308</v>
       </c>
@@ -10218,7 +10249,7 @@
         <v>2.7332754129999999</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
         <v>314</v>
       </c>
@@ -10250,7 +10281,7 @@
         <v>2.6666666669999999</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A55" t="s">
         <v>320</v>
       </c>
@@ -10282,7 +10313,7 @@
         <v>2.626415094</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
         <v>325</v>
       </c>
@@ -10317,7 +10348,7 @@
         <v>2.5333993069999998</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
         <v>332</v>
       </c>
@@ -10352,7 +10383,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
         <v>337</v>
       </c>
@@ -10384,7 +10415,7 @@
         <v>2.3918918919999999</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A59" t="s">
         <v>342</v>
       </c>
@@ -10416,7 +10447,7 @@
         <v>2.3608815430000001</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A60" t="s">
         <v>347</v>
       </c>
@@ -10451,7 +10482,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A61" t="s">
         <v>352</v>
       </c>
@@ -10489,7 +10520,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A62" t="s">
         <v>358</v>
       </c>
@@ -10524,7 +10555,7 @@
         <v>2.1497619920000002</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A63" t="s">
         <v>363</v>
       </c>
@@ -10562,7 +10593,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A64" t="s">
         <v>368</v>
       </c>
@@ -10594,7 +10625,7 @@
         <v>2.0744466799999999</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A65" t="s">
         <v>374</v>
       </c>
@@ -10629,7 +10660,7 @@
         <v>2.0208877279999999</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
         <v>381</v>
       </c>
@@ -10664,7 +10695,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
         <v>385</v>
       </c>
@@ -10696,7 +10727,7 @@
         <v>1.97254902</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A68" t="s">
         <v>391</v>
       </c>
@@ -10731,7 +10762,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A69" t="s">
         <v>397</v>
       </c>
@@ -10769,7 +10800,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A70" t="s">
         <v>403</v>
       </c>
@@ -10804,7 +10835,7 @@
         <v>1.8885779700000001</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A71" t="s">
         <v>410</v>
       </c>
@@ -10836,7 +10867,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A72" t="s">
         <v>415</v>
       </c>
@@ -10868,7 +10899,7 @@
         <v>1.7983193280000001</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A73" t="s">
         <v>421</v>
       </c>
@@ -10906,7 +10937,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A74" t="s">
         <v>428</v>
       </c>
@@ -10938,7 +10969,7 @@
         <v>1.579150579</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A75" t="s">
         <v>434</v>
       </c>
@@ -10970,7 +11001,7 @@
         <v>1.568181818</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A76" t="s">
         <v>439</v>
       </c>
@@ -11002,7 +11033,7 @@
         <v>1.435647584</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A77" t="s">
         <v>445</v>
       </c>
@@ -11037,7 +11068,7 @@
         <v>1.4015724220000001</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A78" t="s">
         <v>451</v>
       </c>
@@ -11069,7 +11100,7 @@
         <v>1.3647798739999999</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A79" t="s">
         <v>455</v>
       </c>
@@ -11101,7 +11132,7 @@
         <v>1.3508403360000001</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A80" t="s">
         <v>461</v>
       </c>
@@ -11133,7 +11164,7 @@
         <v>1.34034824</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A81" t="s">
         <v>467</v>
       </c>
@@ -11168,7 +11199,7 @@
         <v>1.2913669059999999</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A82" t="s">
         <v>473</v>
       </c>
@@ -11203,7 +11234,7 @@
         <v>1.259629101</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A83" t="s">
         <v>479</v>
       </c>
@@ -11235,7 +11266,7 @@
         <v>1.25433526</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A84" t="s">
         <v>485</v>
       </c>
@@ -11270,7 +11301,7 @@
         <v>1.2402420569999999</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A85" t="s">
         <v>491</v>
       </c>
@@ -11302,7 +11333,7 @@
         <v>1.2215113950000001</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A86" t="s">
         <v>497</v>
       </c>
@@ -11337,7 +11368,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A87" t="s">
         <v>503</v>
       </c>
@@ -11369,7 +11400,7 @@
         <v>1.136022514</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A88" t="s">
         <v>508</v>
       </c>
@@ -11401,7 +11432,7 @@
         <v>1.1282633369999999</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A89" t="s">
         <v>514</v>
       </c>
@@ -11433,7 +11464,7 @@
         <v>1.124572211</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A90" t="s">
         <v>520</v>
       </c>
@@ -11462,7 +11493,7 @@
         <v>1.0699300700000001</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A91" t="s">
         <v>525</v>
       </c>
@@ -11491,7 +11522,7 @@
         <v>1.0052083329999999</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A92" t="s">
         <v>530</v>
       </c>
@@ -11526,7 +11557,7 @@
         <v>0.82306752699999997</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A93" t="s">
         <v>535</v>
       </c>
@@ -11558,7 +11589,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A94" t="s">
         <v>540</v>
       </c>
@@ -11572,7 +11603,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A95" t="s">
         <v>543</v>
       </c>
@@ -11583,7 +11614,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A96" t="s">
         <v>545</v>
       </c>
@@ -11606,7 +11637,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A97" t="s">
         <v>550</v>
       </c>
@@ -11629,7 +11660,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A98" t="s">
         <v>555</v>
       </c>
@@ -11652,7 +11683,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A99" t="s">
         <v>559</v>
       </c>
@@ -11675,7 +11706,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A100" t="s">
         <v>563</v>
       </c>
@@ -11698,7 +11729,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A101" t="s">
         <v>568</v>
       </c>
@@ -11721,7 +11752,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A102" t="s">
         <v>572</v>
       </c>
@@ -11744,7 +11775,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A103" t="s">
         <v>577</v>
       </c>
@@ -11767,7 +11798,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A104" t="s">
         <v>582</v>
       </c>
@@ -11790,7 +11821,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A105" t="s">
         <v>585</v>
       </c>
@@ -11813,7 +11844,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A106" t="s">
         <v>589</v>
       </c>
@@ -11830,7 +11861,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.4">
       <c r="C110" s="2"/>
     </row>
   </sheetData>
@@ -11843,10 +11874,10 @@
   <dimension ref="A1:M65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="42.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" customWidth="1"/>
@@ -11854,7 +11885,7 @@
     <col min="5" max="5" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11895,7 +11926,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -11930,7 +11961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -11965,7 +11996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -12000,7 +12031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -12035,7 +12066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -12070,7 +12101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>53</v>
       </c>
@@ -12105,7 +12136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>63</v>
       </c>
@@ -12140,7 +12171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>69</v>
       </c>
@@ -12175,7 +12206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>74</v>
       </c>
@@ -12210,7 +12241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>80</v>
       </c>
@@ -12245,7 +12276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>86</v>
       </c>
@@ -12283,7 +12314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>92</v>
       </c>
@@ -12293,8 +12324,8 @@
       <c r="C13" t="s">
         <v>94</v>
       </c>
-      <c r="D13" s="2">
-        <v>45704</v>
+      <c r="D13" s="2" t="s">
+        <v>655</v>
       </c>
       <c r="E13" t="s">
         <v>95</v>
@@ -12321,7 +12352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>98</v>
       </c>
@@ -12356,7 +12387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>104</v>
       </c>
@@ -12366,8 +12397,8 @@
       <c r="C15" t="s">
         <v>106</v>
       </c>
-      <c r="D15" s="2">
-        <v>45881</v>
+      <c r="D15" s="2" t="s">
+        <v>656</v>
       </c>
       <c r="E15" t="s">
         <v>107</v>
@@ -12394,7 +12425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>110</v>
       </c>
@@ -12404,8 +12435,8 @@
       <c r="C16" t="s">
         <v>112</v>
       </c>
-      <c r="D16" s="2">
-        <v>45719</v>
+      <c r="D16" s="2" t="s">
+        <v>657</v>
       </c>
       <c r="E16" t="s">
         <v>113</v>
@@ -12432,7 +12463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>358</v>
       </c>
@@ -12470,7 +12501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>122</v>
       </c>
@@ -12505,7 +12536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>128</v>
       </c>
@@ -12540,7 +12571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>133</v>
       </c>
@@ -12575,7 +12606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>138</v>
       </c>
@@ -12610,7 +12641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>144</v>
       </c>
@@ -12645,7 +12676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>150</v>
       </c>
@@ -12655,8 +12686,8 @@
       <c r="C23" t="s">
         <v>152</v>
       </c>
-      <c r="D23" s="2">
-        <v>46008</v>
+      <c r="D23" s="2" t="s">
+        <v>658</v>
       </c>
       <c r="E23" t="s">
         <v>153</v>
@@ -12683,7 +12714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>156</v>
       </c>
@@ -12721,7 +12752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>162</v>
       </c>
@@ -12756,7 +12787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>168</v>
       </c>
@@ -12766,8 +12797,8 @@
       <c r="C26" t="s">
         <v>170</v>
       </c>
-      <c r="D26" s="2">
-        <v>45883</v>
+      <c r="D26" s="2" t="s">
+        <v>660</v>
       </c>
       <c r="E26" t="s">
         <v>95</v>
@@ -12794,7 +12825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>207</v>
       </c>
@@ -12829,7 +12860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>212</v>
       </c>
@@ -12864,7 +12895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>241</v>
       </c>
@@ -12902,7 +12933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>248</v>
       </c>
@@ -12937,7 +12968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>254</v>
       </c>
@@ -12972,7 +13003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>260</v>
       </c>
@@ -13007,7 +13038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>272</v>
       </c>
@@ -13017,8 +13048,8 @@
       <c r="C33" t="s">
         <v>274</v>
       </c>
-      <c r="D33" s="2">
-        <v>45822</v>
+      <c r="D33" s="2" t="s">
+        <v>661</v>
       </c>
       <c r="E33" t="s">
         <v>275</v>
@@ -13045,7 +13076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>278</v>
       </c>
@@ -13080,7 +13111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>284</v>
       </c>
@@ -13118,7 +13149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>290</v>
       </c>
@@ -13153,7 +13184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>296</v>
       </c>
@@ -13188,7 +13219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>302</v>
       </c>
@@ -13223,7 +13254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>308</v>
       </c>
@@ -13258,7 +13289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>314</v>
       </c>
@@ -13293,7 +13324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>320</v>
       </c>
@@ -13328,7 +13359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>325</v>
       </c>
@@ -13366,7 +13397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>337</v>
       </c>
@@ -13401,7 +13432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
         <v>342</v>
       </c>
@@ -13436,7 +13467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
         <v>368</v>
       </c>
@@ -13471,7 +13502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
         <v>374</v>
       </c>
@@ -13509,7 +13540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
         <v>11</v>
       </c>
@@ -13544,7 +13575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
         <v>23</v>
       </c>
@@ -13582,7 +13613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
         <v>218</v>
       </c>
@@ -13617,19 +13648,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.4">
       <c r="J50">
         <f>SUM(J2:J46)</f>
         <v>336965</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A51" s="4"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.4">
       <c r="D64" s="2"/>
     </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="4:4" x14ac:dyDescent="0.4">
       <c r="D65" s="2"/>
     </row>
   </sheetData>
@@ -13646,11 +13677,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A02BF73E-DB49-7C43-B649-A3CAA646B49C}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="42.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
@@ -13661,14 +13692,14 @@
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="D1" s="10" t="s">
         <v>645</v>
       </c>
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>649</v>
       </c>
@@ -13691,9 +13722,9 @@
         <v>648</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>207</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
@@ -13714,7 +13745,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -13737,7 +13768,7 @@
         <v>373.64</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -13760,7 +13791,7 @@
         <v>371.75</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -13783,7 +13814,7 @@
         <v>333.4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -13806,7 +13837,7 @@
         <v>198.33333329999999</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -13829,7 +13860,7 @@
         <v>192.58333329999999</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>63</v>
       </c>
@@ -13852,7 +13883,7 @@
         <v>125.16666669999999</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>69</v>
       </c>
@@ -13875,7 +13906,7 @@
         <v>93.92307692</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>74</v>
       </c>
@@ -13898,7 +13929,7 @@
         <v>82.212643679999999</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>80</v>
       </c>
@@ -13921,7 +13952,7 @@
         <v>70.092307689999998</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>86</v>
       </c>
@@ -13944,7 +13975,7 @@
         <v>61.446153850000002</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>92</v>
       </c>
@@ -13967,7 +13998,7 @@
         <v>52.433155079999999</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>98</v>
       </c>
@@ -13990,7 +14021,7 @@
         <v>38.024390240000002</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>104</v>
       </c>
@@ -14013,7 +14044,7 @@
         <v>31.38356164</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>110</v>
       </c>
@@ -14036,7 +14067,7 @@
         <v>26.13839286</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>358</v>
       </c>
@@ -14059,7 +14090,7 @@
         <v>2.1497619920000002</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>122</v>
       </c>
@@ -14082,7 +14113,7 @@
         <v>21.704724410000001</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>128</v>
       </c>
@@ -14105,7 +14136,7 @@
         <v>17.571428569999998</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>133</v>
       </c>
@@ -14128,7 +14159,7 @@
         <v>15.289908260000001</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>138</v>
       </c>
@@ -14151,7 +14182,7 @@
         <v>13.29032258</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>144</v>
       </c>
@@ -14174,7 +14205,7 @@
         <v>11.27737226</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>150</v>
       </c>
@@ -14197,7 +14228,7 @@
         <v>10.741427249999999</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>156</v>
       </c>
@@ -14220,7 +14251,7 @@
         <v>9.4833272260000001</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>162</v>
       </c>
@@ -14243,7 +14274,7 @@
         <v>9.461538462</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>168</v>
       </c>
@@ -14266,7 +14297,7 @@
         <v>9.4278169009999999</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>207</v>
       </c>
@@ -14289,7 +14320,7 @@
         <v>5.6666666670000003</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>212</v>
       </c>
@@ -14312,7 +14343,7 @@
         <v>5.4341463409999999</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>241</v>
       </c>
@@ -14335,7 +14366,7 @@
         <v>4.4124168509999997</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>248</v>
       </c>
@@ -14358,7 +14389,7 @@
         <v>4.1982507289999997</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>254</v>
       </c>
@@ -14381,7 +14412,7 @@
         <v>4.0868644070000002</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>260</v>
       </c>
@@ -14404,7 +14435,7 @@
         <v>4.0077519380000002</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>272</v>
       </c>
@@ -14427,7 +14458,7 @@
         <v>3.6413934430000001</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>278</v>
       </c>
@@ -14450,7 +14481,7 @@
         <v>3.5825825830000002</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>284</v>
       </c>
@@ -14473,7 +14504,7 @@
         <v>3.404090268</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>290</v>
       </c>
@@ -14496,7 +14527,7 @@
         <v>3.1278608480000001</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>296</v>
       </c>
@@ -14519,7 +14550,7 @@
         <v>3.074449666</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>302</v>
       </c>
@@ -14542,7 +14573,7 @@
         <v>2.9500594530000002</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>308</v>
       </c>
@@ -14565,7 +14596,7 @@
         <v>2.7332754129999999</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>314</v>
       </c>
@@ -14588,7 +14619,7 @@
         <v>2.6666666669999999</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>320</v>
       </c>
@@ -14611,7 +14642,7 @@
         <v>2.626415094</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>325</v>
       </c>
@@ -14634,7 +14665,7 @@
         <v>2.5333993069999998</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
         <v>337</v>
       </c>
@@ -14657,7 +14688,7 @@
         <v>2.3918918919999999</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
         <v>342</v>
       </c>
@@ -14680,7 +14711,7 @@
         <v>2.3608815430000001</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
         <v>368</v>
       </c>
@@ -14703,7 +14734,7 @@
         <v>2.0744466799999999</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
         <v>374</v>
       </c>
@@ -14726,7 +14757,7 @@
         <v>2.0208877279999999</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
         <v>11</v>
       </c>
@@ -14749,7 +14780,7 @@
         <v>732.06896549999999</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
         <v>23</v>
       </c>
@@ -14772,7 +14803,7 @@
         <v>374.1935484</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
         <v>218</v>
       </c>
@@ -14795,7 +14826,7 @@
         <v>5.0028715000000004</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.4">
       <c r="F51">
         <f>SUM(F3:F47,F48,F50)</f>
         <v>386394</v>
@@ -14820,6 +14851,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7cc633b7-a0d7-44f6-9ebf-b0bcc1d1386b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f1ebdc78-f2a0-4ed8-b1e0-396e97b61f03" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002E9A67939B0F2B4787EAA086EFF368F8" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="19bc27e53486324854919c033e632552">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7cc633b7-a0d7-44f6-9ebf-b0bcc1d1386b" xmlns:ns3="f1ebdc78-f2a0-4ed8-b1e0-396e97b61f03" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f11af0e2bfcf2c17163fcf1c9e67185e" ns2:_="" ns3:_="">
     <xsd:import namespace="7cc633b7-a0d7-44f6-9ebf-b0bcc1d1386b"/>
@@ -15026,17 +15068,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7cc633b7-a0d7-44f6-9ebf-b0bcc1d1386b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f1ebdc78-f2a0-4ed8-b1e0-396e97b61f03" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8453017-20DB-4925-80CE-81169A5B0924}">
   <ds:schemaRefs>
@@ -15046,6 +15077,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9CF910F-97D5-44CE-8C0C-659BCA9179A3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7cc633b7-a0d7-44f6-9ebf-b0bcc1d1386b"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="f1ebdc78-f2a0-4ed8-b1e0-396e97b61f03"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8C91DF3-97A4-4305-A107-ECAA15ED5F78}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15062,21 +15110,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9CF910F-97D5-44CE-8C0C-659BCA9179A3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7cc633b7-a0d7-44f6-9ebf-b0bcc1d1386b"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="f1ebdc78-f2a0-4ed8-b1e0-396e97b61f03"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>